<commit_message>
added printAll data, small rework singleton
</commit_message>
<xml_diff>
--- a/src/main/resources/report1.xlsx
+++ b/src/main/resources/report1.xlsx
@@ -12,20 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Kwiatek</t>
-  </si>
-  <si>
-    <t>Mariusz</t>
-  </si>
-  <si>
-    <t>Kwiatkowski</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68,35 +55,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="n">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="n">
-        <v>9.5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>